<commit_message>
Need to Add Function in DataTable Format
</commit_message>
<xml_diff>
--- a/Input/My Logic Excel.xlsx
+++ b/Input/My Logic Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\UiPath\SodexoProcess\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2778E45-4995-4267-AA3D-75AC0311A915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5328835-8E30-4960-9268-3F44ED40131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2810,11 +2810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D742BF-D277-4657-84BB-A3DD0282270A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A541" workbookViewId="0">
-      <selection activeCell="A579" sqref="A579"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3133,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>31009631</v>
       </c>
@@ -3163,7 +3162,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>31009631</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>31009631</v>
       </c>
@@ -3223,7 +3222,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>31009631</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>82300122</v>
       </c>
@@ -3283,7 +3282,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>82300122</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>31009631</v>
       </c>
@@ -3643,7 +3642,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>31009631</v>
       </c>
@@ -3673,7 +3672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>31009631</v>
       </c>
@@ -3703,7 +3702,7 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>31009631</v>
       </c>
@@ -3733,7 +3732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>82400114</v>
       </c>
@@ -3763,7 +3762,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>82400114</v>
       </c>
@@ -3793,7 +3792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31009631</v>
       </c>
@@ -3823,7 +3822,7 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31009631</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31009631</v>
       </c>
@@ -3883,7 +3882,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>31009631</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>31009631</v>
       </c>
@@ -3943,7 +3942,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>31009631</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>31009631</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>31009631</v>
       </c>
@@ -4033,7 +4032,7 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>31009631</v>
       </c>
@@ -4123,7 +4122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>31009631</v>
       </c>
@@ -4153,7 +4152,7 @@
       </c>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>31009631</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>22111711</v>
       </c>
@@ -4213,7 +4212,7 @@
       </c>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>22111711</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>82400114</v>
       </c>
@@ -4273,7 +4272,7 @@
       </c>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>82400114</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>82400199</v>
       </c>
@@ -4333,7 +4332,7 @@
       </c>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>82400199</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>99000000</v>
       </c>
@@ -4393,7 +4392,7 @@
       </c>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>99000000</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>22111711</v>
       </c>
@@ -4453,7 +4452,7 @@
       </c>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>22111711</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>81600118</v>
       </c>
@@ -4573,7 +4572,7 @@
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>81600118</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>31009631</v>
       </c>
@@ -4873,7 +4872,7 @@
       </c>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>31009631</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>31009631</v>
       </c>
@@ -4933,7 +4932,7 @@
       </c>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>31009631</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>82300122</v>
       </c>
@@ -4993,7 +4992,7 @@
       </c>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>82300122</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>82400114</v>
       </c>
@@ -5053,7 +5052,7 @@
       </c>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>82400114</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>82400114</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>25004111</v>
       </c>
@@ -5143,7 +5142,7 @@
       </c>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>25004111</v>
       </c>
@@ -5293,7 +5292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>31009631</v>
       </c>
@@ -5323,7 +5322,7 @@
       </c>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>31009631</v>
       </c>
@@ -5353,7 +5352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>25001611</v>
       </c>
@@ -5383,7 +5382,7 @@
       </c>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>25001611</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43014831</v>
       </c>
@@ -5443,7 +5442,7 @@
       </c>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43014831</v>
       </c>
@@ -5473,7 +5472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>25003511</v>
       </c>
@@ -5503,7 +5502,7 @@
       </c>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>25003511</v>
       </c>
@@ -5533,7 +5532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>31009631</v>
       </c>
@@ -5563,7 +5562,7 @@
       </c>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>31009631</v>
       </c>
@@ -5593,7 +5592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>31009631</v>
       </c>
@@ -5623,7 +5622,7 @@
       </c>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>31009631</v>
       </c>
@@ -5713,7 +5712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>15004111</v>
       </c>
@@ -5743,7 +5742,7 @@
       </c>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>15004111</v>
       </c>
@@ -5773,7 +5772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>31009631</v>
       </c>
@@ -5803,7 +5802,7 @@
       </c>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>31009631</v>
       </c>
@@ -5833,7 +5832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>31009631</v>
       </c>
@@ -5863,7 +5862,7 @@
       </c>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>31009631</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>31009631</v>
       </c>
@@ -5923,7 +5922,7 @@
       </c>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>31009631</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>31009631</v>
       </c>
@@ -6043,7 +6042,7 @@
       </c>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>31009631</v>
       </c>
@@ -6073,7 +6072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>31009631</v>
       </c>
@@ -6103,7 +6102,7 @@
       </c>
       <c r="J109" s="2"/>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>31009631</v>
       </c>
@@ -6133,7 +6132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>31009631</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>42123231</v>
       </c>
@@ -6193,7 +6192,7 @@
       </c>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>42123231</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>42123231</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>31009631</v>
       </c>
@@ -6283,7 +6282,7 @@
       </c>
       <c r="J115" s="2"/>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>31009631</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43020141</v>
       </c>
@@ -6343,7 +6342,7 @@
       </c>
       <c r="J117" s="2"/>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43020141</v>
       </c>
@@ -6373,7 +6372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>43020141</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>31009631</v>
       </c>
@@ -6433,7 +6432,7 @@
       </c>
       <c r="J120" s="2"/>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>31009631</v>
       </c>
@@ -7783,7 +7782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>25007302</v>
       </c>
@@ -7813,7 +7812,7 @@
       </c>
       <c r="J166" s="2"/>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>25007302</v>
       </c>
@@ -7903,7 +7902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>81600118</v>
       </c>
@@ -7933,7 +7932,7 @@
       </c>
       <c r="J170" s="2"/>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>81600118</v>
       </c>
@@ -7963,7 +7962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>82400120</v>
       </c>
@@ -7993,7 +7992,7 @@
       </c>
       <c r="J172" s="2"/>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>82400120</v>
       </c>
@@ -8563,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>54007711</v>
       </c>
@@ -8623,7 +8622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>41007711</v>
       </c>
@@ -8653,7 +8652,7 @@
       </c>
       <c r="J194" s="2"/>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>41007711</v>
       </c>
@@ -9043,7 +9042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>54007711</v>
       </c>
@@ -9253,7 +9252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>41012411</v>
       </c>
@@ -9283,7 +9282,7 @@
       </c>
       <c r="J215" s="2"/>
     </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>41012411</v>
       </c>
@@ -9313,7 +9312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>31009631</v>
       </c>
@@ -9343,7 +9342,7 @@
       </c>
       <c r="J217" s="2"/>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>31009631</v>
       </c>
@@ -9373,7 +9372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>80700156</v>
       </c>
@@ -9403,7 +9402,7 @@
       </c>
       <c r="J219" s="2"/>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>80700156</v>
       </c>
@@ -9433,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>31009631</v>
       </c>
@@ -9463,7 +9462,7 @@
       </c>
       <c r="J221" s="2"/>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>31009631</v>
       </c>
@@ -9553,7 +9552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>21044411</v>
       </c>
@@ -9583,7 +9582,7 @@
       </c>
       <c r="J225" s="2"/>
     </row>
-    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>21044411</v>
       </c>
@@ -9613,7 +9612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>82400115</v>
       </c>
@@ -9643,7 +9642,7 @@
       </c>
       <c r="J227" s="2"/>
     </row>
-    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>82400115</v>
       </c>
@@ -9733,7 +9732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>22111911</v>
       </c>
@@ -9763,7 +9762,7 @@
       </c>
       <c r="J231" s="2"/>
     </row>
-    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>22111911</v>
       </c>
@@ -9793,7 +9792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>41031711</v>
       </c>
@@ -9823,7 +9822,7 @@
       </c>
       <c r="J233" s="2"/>
     </row>
-    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>41031711</v>
       </c>
@@ -9853,7 +9852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>41031711</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>41031711</v>
       </c>
@@ -9913,7 +9912,7 @@
       </c>
       <c r="J236" s="2"/>
     </row>
-    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>41031711</v>
       </c>
@@ -10363,7 +10362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>54007711</v>
       </c>
@@ -10423,7 +10422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>41031711</v>
       </c>
@@ -10453,7 +10452,7 @@
       </c>
       <c r="J254" s="2"/>
     </row>
-    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>41031711</v>
       </c>
@@ -10543,7 +10542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>82400115</v>
       </c>
@@ -10573,7 +10572,7 @@
       </c>
       <c r="J258" s="2"/>
     </row>
-    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>82400115</v>
       </c>
@@ -10663,7 +10662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>80100134</v>
       </c>
@@ -10693,7 +10692,7 @@
       </c>
       <c r="J262" s="2"/>
     </row>
-    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>80100134</v>
       </c>
@@ -10723,7 +10722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>82400104</v>
       </c>
@@ -10753,7 +10752,7 @@
       </c>
       <c r="J264" s="2"/>
     </row>
-    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>82400104</v>
       </c>
@@ -10783,7 +10782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>82400108</v>
       </c>
@@ -10813,7 +10812,7 @@
       </c>
       <c r="J266" s="2"/>
     </row>
-    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>82400108</v>
       </c>
@@ -10933,7 +10932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>25008111</v>
       </c>
@@ -10963,7 +10962,7 @@
       </c>
       <c r="J271" s="2"/>
     </row>
-    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>25008111</v>
       </c>
@@ -10993,7 +10992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="273" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>41008531</v>
       </c>
@@ -11023,7 +11022,7 @@
       </c>
       <c r="J273" s="2"/>
     </row>
-    <row r="274" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>41008531</v>
       </c>
@@ -11053,7 +11052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>31009631</v>
       </c>
@@ -11083,7 +11082,7 @@
       </c>
       <c r="J275" s="2"/>
     </row>
-    <row r="276" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>31009631</v>
       </c>
@@ -11113,7 +11112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="277" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="12">
         <v>99000000</v>
       </c>
@@ -11143,7 +11142,7 @@
       </c>
       <c r="J277" s="13"/>
     </row>
-    <row r="278" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="12">
         <v>99000000</v>
       </c>
@@ -11173,7 +11172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="279" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="12">
         <v>99000000</v>
       </c>
@@ -11203,7 +11202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="280" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="12">
         <v>99000000</v>
       </c>
@@ -11233,7 +11232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="12">
         <v>99000000</v>
       </c>
@@ -11263,7 +11262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="282" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>15004111</v>
       </c>
@@ -11293,7 +11292,7 @@
       </c>
       <c r="J282" s="2"/>
     </row>
-    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>15004111</v>
       </c>
@@ -11323,7 +11322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>82400124</v>
       </c>
@@ -11353,7 +11352,7 @@
       </c>
       <c r="J284" s="2"/>
     </row>
-    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>82400124</v>
       </c>
@@ -11383,7 +11382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="286" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>22112011</v>
       </c>
@@ -11413,7 +11412,7 @@
       </c>
       <c r="J286" s="2"/>
     </row>
-    <row r="287" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>22112011</v>
       </c>
@@ -11443,7 +11442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>31009631</v>
       </c>
@@ -11473,7 +11472,7 @@
       </c>
       <c r="J288" s="2"/>
     </row>
-    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>31009631</v>
       </c>
@@ -11503,7 +11502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="4">
         <v>41008531</v>
       </c>
@@ -11533,7 +11532,7 @@
       </c>
       <c r="J290" s="5"/>
     </row>
-    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="4">
         <v>41008531</v>
       </c>
@@ -11563,7 +11562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="4">
         <v>41008531</v>
       </c>
@@ -11593,7 +11592,7 @@
       </c>
       <c r="J292" s="5"/>
     </row>
-    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="4">
         <v>41008531</v>
       </c>
@@ -11623,7 +11622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="4">
         <v>41008531</v>
       </c>
@@ -11653,7 +11652,7 @@
       </c>
       <c r="J294" s="5"/>
     </row>
-    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="4">
         <v>41008531</v>
       </c>
@@ -11683,7 +11682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>41008531</v>
       </c>
@@ -11713,7 +11712,7 @@
       </c>
       <c r="J296" s="2"/>
     </row>
-    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>41008531</v>
       </c>
@@ -11833,7 +11832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>31009631</v>
       </c>
@@ -11863,7 +11862,7 @@
       </c>
       <c r="J301" s="2"/>
     </row>
-    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>31009631</v>
       </c>
@@ -11893,7 +11892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>31009631</v>
       </c>
@@ -11923,7 +11922,7 @@
       </c>
       <c r="J303" s="2"/>
     </row>
-    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>31009631</v>
       </c>
@@ -12073,7 +12072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>31009631</v>
       </c>
@@ -12103,7 +12102,7 @@
       </c>
       <c r="J309" s="2"/>
     </row>
-    <row r="310" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>31009631</v>
       </c>
@@ -12133,7 +12132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="311" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>31009631</v>
       </c>
@@ -12163,7 +12162,7 @@
       </c>
       <c r="J311" s="2"/>
     </row>
-    <row r="312" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>31009631</v>
       </c>
@@ -12193,7 +12192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>15004111</v>
       </c>
@@ -12223,7 +12222,7 @@
       </c>
       <c r="J313" s="2"/>
     </row>
-    <row r="314" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>15004111</v>
       </c>
@@ -12253,7 +12252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="315" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>31009631</v>
       </c>
@@ -12283,7 +12282,7 @@
       </c>
       <c r="J315" s="2"/>
     </row>
-    <row r="316" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>31009631</v>
       </c>
@@ -12313,7 +12312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="317" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>31009631</v>
       </c>
@@ -12343,7 +12342,7 @@
       </c>
       <c r="J317" s="2"/>
     </row>
-    <row r="318" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>31009631</v>
       </c>
@@ -12493,7 +12492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="323" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>31009631</v>
       </c>
@@ -12523,7 +12522,7 @@
       </c>
       <c r="J323" s="2"/>
     </row>
-    <row r="324" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>31009631</v>
       </c>
@@ -12553,7 +12552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="325" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>31009631</v>
       </c>
@@ -12583,7 +12582,7 @@
       </c>
       <c r="J325" s="2"/>
     </row>
-    <row r="326" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>31009631</v>
       </c>
@@ -12673,7 +12672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="329" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>31009631</v>
       </c>
@@ -12703,7 +12702,7 @@
       </c>
       <c r="J329" s="2"/>
     </row>
-    <row r="330" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>31009631</v>
       </c>
@@ -12733,7 +12732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="331" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>31009631</v>
       </c>
@@ -12763,7 +12762,7 @@
       </c>
       <c r="J331" s="2"/>
     </row>
-    <row r="332" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>31009631</v>
       </c>
@@ -12793,7 +12792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="333" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>81600116</v>
       </c>
@@ -12823,7 +12822,7 @@
       </c>
       <c r="J333" s="2"/>
     </row>
-    <row r="334" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>81600116</v>
       </c>
@@ -12913,7 +12912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="337" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>80100133</v>
       </c>
@@ -12943,7 +12942,7 @@
       </c>
       <c r="J337" s="2"/>
     </row>
-    <row r="338" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>80100133</v>
       </c>
@@ -12973,7 +12972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="339" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>35012511</v>
       </c>
@@ -13003,7 +13002,7 @@
       </c>
       <c r="J339" s="2"/>
     </row>
-    <row r="340" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>35012511</v>
       </c>
@@ -13033,7 +13032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" s="4">
         <v>41008531</v>
       </c>
@@ -13063,7 +13062,7 @@
       </c>
       <c r="J341" s="5"/>
     </row>
-    <row r="342" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="4">
         <v>41008531</v>
       </c>
@@ -13093,7 +13092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>31009631</v>
       </c>
@@ -13123,7 +13122,7 @@
       </c>
       <c r="J343" s="2"/>
     </row>
-    <row r="344" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>31009631</v>
       </c>
@@ -13213,7 +13212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="347" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>80700109</v>
       </c>
@@ -13243,7 +13242,7 @@
       </c>
       <c r="J347" s="2"/>
     </row>
-    <row r="348" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>80700109</v>
       </c>
@@ -13273,7 +13272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="349" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>80700109</v>
       </c>
@@ -13303,7 +13302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="350" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>80700109</v>
       </c>
@@ -13333,7 +13332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="351" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>80700109</v>
       </c>
@@ -13363,7 +13362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="352" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>31108511</v>
       </c>
@@ -13393,7 +13392,7 @@
       </c>
       <c r="J352" s="2"/>
     </row>
-    <row r="353" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>31108511</v>
       </c>
@@ -13423,7 +13422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="354" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>31108511</v>
       </c>
@@ -13453,7 +13452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>36001431</v>
       </c>
@@ -13483,7 +13482,7 @@
       </c>
       <c r="J355" s="2"/>
     </row>
-    <row r="356" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>36001431</v>
       </c>
@@ -13513,7 +13512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="357" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>36001431</v>
       </c>
@@ -13603,7 +13602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="360" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>31009631</v>
       </c>
@@ -13633,7 +13632,7 @@
       </c>
       <c r="J360" s="2"/>
     </row>
-    <row r="361" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>31009631</v>
       </c>
@@ -13663,7 +13662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="362" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>31009631</v>
       </c>
@@ -13693,7 +13692,7 @@
       </c>
       <c r="J362" s="2"/>
     </row>
-    <row r="363" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>31009631</v>
       </c>
@@ -13723,7 +13722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>80700103</v>
       </c>
@@ -13753,7 +13752,7 @@
       </c>
       <c r="J364" s="2"/>
     </row>
-    <row r="365" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>80700103</v>
       </c>
@@ -13783,7 +13782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="366" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>80700103</v>
       </c>
@@ -13813,7 +13812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>31009631</v>
       </c>
@@ -13843,7 +13842,7 @@
       </c>
       <c r="J367" s="2"/>
     </row>
-    <row r="368" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>31009631</v>
       </c>
@@ -13873,7 +13872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="369" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>31009631</v>
       </c>
@@ -13903,7 +13902,7 @@
       </c>
       <c r="J369" s="2"/>
     </row>
-    <row r="370" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>31009631</v>
       </c>
@@ -13933,7 +13932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>31009631</v>
       </c>
@@ -13963,7 +13962,7 @@
       </c>
       <c r="J371" s="2"/>
     </row>
-    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>31009631</v>
       </c>
@@ -13993,7 +13992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="373" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>31009631</v>
       </c>
@@ -14023,7 +14022,7 @@
       </c>
       <c r="J373" s="2"/>
     </row>
-    <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>31009631</v>
       </c>
@@ -14053,7 +14052,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>31009631</v>
       </c>
@@ -14083,7 +14082,7 @@
       </c>
       <c r="J375" s="2"/>
     </row>
-    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>31009631</v>
       </c>
@@ -14473,7 +14472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>80800102</v>
       </c>
@@ -14503,7 +14502,7 @@
       </c>
       <c r="J389" s="2"/>
     </row>
-    <row r="390" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>80800102</v>
       </c>
@@ -14653,7 +14652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="395" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>41040311</v>
       </c>
@@ -14683,7 +14682,7 @@
       </c>
       <c r="J395" s="2"/>
     </row>
-    <row r="396" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>41040311</v>
       </c>
@@ -14713,7 +14712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="397" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>43015631</v>
       </c>
@@ -14743,7 +14742,7 @@
       </c>
       <c r="J397" s="2"/>
     </row>
-    <row r="398" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>43015631</v>
       </c>
@@ -14773,7 +14772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="399" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>22112211</v>
       </c>
@@ -14803,7 +14802,7 @@
       </c>
       <c r="J399" s="2"/>
     </row>
-    <row r="400" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>22112211</v>
       </c>
@@ -14833,7 +14832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="401" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>43029311</v>
       </c>
@@ -14863,7 +14862,7 @@
       </c>
       <c r="J401" s="2"/>
     </row>
-    <row r="402" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>43029311</v>
       </c>
@@ -14893,7 +14892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="403" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>43016431</v>
       </c>
@@ -14923,7 +14922,7 @@
       </c>
       <c r="J403" s="2"/>
     </row>
-    <row r="404" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>43016431</v>
       </c>
@@ -14953,7 +14952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="405" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>41012411</v>
       </c>
@@ -14983,7 +14982,7 @@
       </c>
       <c r="J405" s="2"/>
     </row>
-    <row r="406" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>41012411</v>
       </c>
@@ -15313,7 +15312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="417" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>82400145</v>
       </c>
@@ -15343,7 +15342,7 @@
       </c>
       <c r="J417" s="2"/>
     </row>
-    <row r="418" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>82400145</v>
       </c>
@@ -15433,7 +15432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="421" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>21040711</v>
       </c>
@@ -15463,7 +15462,7 @@
       </c>
       <c r="J421" s="2"/>
     </row>
-    <row r="422" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>21040711</v>
       </c>
@@ -15493,7 +15492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="423" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>31009631</v>
       </c>
@@ -15523,7 +15522,7 @@
       </c>
       <c r="J423" s="2"/>
     </row>
-    <row r="424" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>31009631</v>
       </c>
@@ -15553,7 +15552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="425" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>31009631</v>
       </c>
@@ -15583,7 +15582,7 @@
       </c>
       <c r="J425" s="2"/>
     </row>
-    <row r="426" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>31009631</v>
       </c>
@@ -15853,7 +15852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="435" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>15004111</v>
       </c>
@@ -15883,7 +15882,7 @@
       </c>
       <c r="J435" s="2"/>
     </row>
-    <row r="436" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>15004111</v>
       </c>
@@ -15913,7 +15912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="437" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>90100002</v>
       </c>
@@ -15943,7 +15942,7 @@
       </c>
       <c r="J437" s="2"/>
     </row>
-    <row r="438" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>90100002</v>
       </c>
@@ -15973,7 +15972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="439" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>81800111</v>
       </c>
@@ -16003,7 +16002,7 @@
       </c>
       <c r="J439" s="2"/>
     </row>
-    <row r="440" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>81800111</v>
       </c>
@@ -16033,7 +16032,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="441" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>81800111</v>
       </c>
@@ -16063,7 +16062,7 @@
       </c>
       <c r="J441" s="2"/>
     </row>
-    <row r="442" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>81800111</v>
       </c>
@@ -16153,7 +16152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="445" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>81800111</v>
       </c>
@@ -16183,7 +16182,7 @@
       </c>
       <c r="J445" s="2"/>
     </row>
-    <row r="446" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>81800111</v>
       </c>
@@ -16273,7 +16272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="449" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>21041611</v>
       </c>
@@ -16303,7 +16302,7 @@
       </c>
       <c r="J449" s="2"/>
     </row>
-    <row r="450" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>21041611</v>
       </c>
@@ -16393,7 +16392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="453" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>81800102</v>
       </c>
@@ -16423,7 +16422,7 @@
       </c>
       <c r="J453" s="2"/>
     </row>
-    <row r="454" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>81800102</v>
       </c>
@@ -16453,7 +16452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="455" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>81800118</v>
       </c>
@@ -16483,7 +16482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="456" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>81800109</v>
       </c>
@@ -16513,7 +16512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="457" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>81800111</v>
       </c>
@@ -16543,7 +16542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="458" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>81800110</v>
       </c>
@@ -16573,7 +16572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>81800124</v>
       </c>
@@ -16603,7 +16602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="460" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>81800112</v>
       </c>
@@ -16633,7 +16632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="461" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>81800115</v>
       </c>
@@ -16663,7 +16662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="462" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>81800107</v>
       </c>
@@ -16693,7 +16692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>81800106</v>
       </c>
@@ -16723,7 +16722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="464" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>81800104</v>
       </c>
@@ -16753,7 +16752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="465" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>81800113</v>
       </c>
@@ -16783,7 +16782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="466" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>80800109</v>
       </c>
@@ -16813,7 +16812,7 @@
       </c>
       <c r="J466" s="2"/>
     </row>
-    <row r="467" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>80800109</v>
       </c>
@@ -16843,7 +16842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="468" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>80800118</v>
       </c>
@@ -16873,7 +16872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="469" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>80800104</v>
       </c>
@@ -16903,7 +16902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="470" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>80800111</v>
       </c>
@@ -16933,7 +16932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="471" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>80800112</v>
       </c>
@@ -16963,7 +16962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="472" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>80800127</v>
       </c>
@@ -16993,7 +16992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="473" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>80800115</v>
       </c>
@@ -17023,7 +17022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="474" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>82300123</v>
       </c>
@@ -17053,7 +17052,7 @@
       </c>
       <c r="J474" s="2"/>
     </row>
-    <row r="475" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>82300123</v>
       </c>
@@ -17083,7 +17082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="476" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>31009631</v>
       </c>
@@ -17113,7 +17112,7 @@
       </c>
       <c r="J476" s="2"/>
     </row>
-    <row r="477" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>31009631</v>
       </c>
@@ -17143,7 +17142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="478" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>81200118</v>
       </c>
@@ -17173,7 +17172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="479" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>81200110</v>
       </c>
@@ -17203,7 +17202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="480" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>81200102</v>
       </c>
@@ -17233,7 +17232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="481" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>81200104</v>
       </c>
@@ -17383,7 +17382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="486" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <v>81100117</v>
       </c>
@@ -17413,7 +17412,7 @@
       </c>
       <c r="J486" s="2"/>
     </row>
-    <row r="487" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <v>81100117</v>
       </c>
@@ -17443,7 +17442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="488" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <v>81100118</v>
       </c>
@@ -17473,7 +17472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="489" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A489" s="1">
         <v>81100109</v>
       </c>
@@ -17503,7 +17502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="490" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A490" s="1">
         <v>81100110</v>
       </c>
@@ -17533,7 +17532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="491" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A491" s="1">
         <v>81100112</v>
       </c>
@@ -17563,7 +17562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="492" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>81100134</v>
       </c>
@@ -17593,7 +17592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="493" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <v>81100102</v>
       </c>
@@ -17623,7 +17622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="494" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A494" s="1">
         <v>81100104</v>
       </c>
@@ -17653,7 +17652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="495" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <v>81100115</v>
       </c>
@@ -17683,7 +17682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="496" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A496" s="1">
         <v>81100106</v>
       </c>
@@ -17773,7 +17772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="499" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A499" s="1">
         <v>81600111</v>
       </c>
@@ -17803,7 +17802,7 @@
       </c>
       <c r="J499" s="2"/>
     </row>
-    <row r="500" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A500" s="1">
         <v>81600111</v>
       </c>
@@ -17833,7 +17832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="501" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A501" s="1">
         <v>81600118</v>
       </c>
@@ -17863,7 +17862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="502" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A502" s="1">
         <v>81600128</v>
       </c>
@@ -17893,7 +17892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="503" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A503" s="1">
         <v>81600102</v>
       </c>
@@ -17923,7 +17922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="504" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A504" s="1">
         <v>81600109</v>
       </c>
@@ -17953,7 +17952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="505" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A505" s="1">
         <v>81600107</v>
       </c>
@@ -17983,7 +17982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="506" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <v>81600110</v>
       </c>
@@ -18013,7 +18012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="507" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A507" s="1">
         <v>81600115</v>
       </c>
@@ -18043,7 +18042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="508" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A508" s="1">
         <v>81600113</v>
       </c>
@@ -18073,7 +18072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="509" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A509" s="1">
         <v>81600112</v>
       </c>
@@ -18103,7 +18102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="510" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A510" s="1">
         <v>82200127</v>
       </c>
@@ -18133,7 +18132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="511" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A511" s="1">
         <v>82400182</v>
       </c>
@@ -18163,7 +18162,7 @@
       </c>
       <c r="J511" s="2"/>
     </row>
-    <row r="512" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A512" s="1">
         <v>82400182</v>
       </c>
@@ -18193,7 +18192,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="513" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A513" s="4">
         <v>80100133</v>
       </c>
@@ -18223,7 +18222,7 @@
       </c>
       <c r="J513" s="5"/>
     </row>
-    <row r="514" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A514" s="4">
         <v>80100133</v>
       </c>
@@ -18253,7 +18252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="515" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A515" s="4">
         <v>80100133</v>
       </c>
@@ -18283,7 +18282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A516" s="1">
         <v>31009631</v>
       </c>
@@ -18313,7 +18312,7 @@
       </c>
       <c r="J516" s="2"/>
     </row>
-    <row r="517" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A517" s="1">
         <v>31009631</v>
       </c>
@@ -18343,7 +18342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="518" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A518" s="1">
         <v>31009631</v>
       </c>
@@ -18373,7 +18372,7 @@
       </c>
       <c r="J518" s="2"/>
     </row>
-    <row r="519" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A519" s="1">
         <v>31009631</v>
       </c>
@@ -18403,7 +18402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="520" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A520" s="1">
         <v>31009631</v>
       </c>
@@ -18433,7 +18432,7 @@
       </c>
       <c r="J520" s="2"/>
     </row>
-    <row r="521" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A521" s="1">
         <v>31009631</v>
       </c>
@@ -18463,7 +18462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="522" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A522" s="1">
         <v>31009631</v>
       </c>
@@ -18493,7 +18492,7 @@
       </c>
       <c r="J522" s="2"/>
     </row>
-    <row r="523" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A523" s="1">
         <v>31009631</v>
       </c>
@@ -18523,7 +18522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="524" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A524" s="1">
         <v>31009631</v>
       </c>
@@ -18553,7 +18552,7 @@
       </c>
       <c r="J524" s="2"/>
     </row>
-    <row r="525" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A525" s="1">
         <v>31009631</v>
       </c>
@@ -18583,7 +18582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="526" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A526" s="1">
         <v>31009631</v>
       </c>
@@ -18613,7 +18612,7 @@
       </c>
       <c r="J526" s="2"/>
     </row>
-    <row r="527" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A527" s="1">
         <v>31009631</v>
       </c>
@@ -18643,7 +18642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="528" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A528" s="1">
         <v>15004111</v>
       </c>
@@ -18673,7 +18672,7 @@
       </c>
       <c r="J528" s="2"/>
     </row>
-    <row r="529" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A529" s="1">
         <v>15004111</v>
       </c>
@@ -18883,7 +18882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="536" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A536" s="1">
         <v>31009631</v>
       </c>
@@ -18913,7 +18912,7 @@
       </c>
       <c r="J536" s="2"/>
     </row>
-    <row r="537" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A537" s="1">
         <v>31009631</v>
       </c>
@@ -18943,7 +18942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="538" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A538" s="1">
         <v>31009631</v>
       </c>
@@ -18973,7 +18972,7 @@
       </c>
       <c r="J538" s="2"/>
     </row>
-    <row r="539" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A539" s="1">
         <v>31009631</v>
       </c>
@@ -19153,7 +19152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="545" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A545" s="17">
         <v>42014931</v>
       </c>
@@ -19183,7 +19182,7 @@
       </c>
       <c r="J545" s="15"/>
     </row>
-    <row r="546" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A546" s="17">
         <v>42014931</v>
       </c>
@@ -19213,7 +19212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="547" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A547" s="17">
         <v>42014931</v>
       </c>
@@ -19243,7 +19242,7 @@
       </c>
       <c r="J547" s="15"/>
     </row>
-    <row r="548" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A548" s="17">
         <v>42014931</v>
       </c>
@@ -19273,7 +19272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="549" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A549" s="17">
         <v>42014931</v>
       </c>
@@ -19303,7 +19302,7 @@
       </c>
       <c r="J549" s="15"/>
     </row>
-    <row r="550" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A550" s="17">
         <v>42014931</v>
       </c>
@@ -19333,7 +19332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="551" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A551" s="17">
         <v>82400125</v>
       </c>
@@ -19363,7 +19362,7 @@
       </c>
       <c r="J551" s="15"/>
     </row>
-    <row r="552" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A552" s="17">
         <v>82400125</v>
       </c>
@@ -19933,7 +19932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="571" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A571" s="20">
         <v>32003711</v>
       </c>
@@ -19963,7 +19962,7 @@
       </c>
       <c r="J571" s="21"/>
     </row>
-    <row r="572" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A572" s="20">
         <v>32003711</v>
       </c>
@@ -19993,7 +19992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="573" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A573" s="20">
         <v>32003711</v>
       </c>
@@ -20023,7 +20022,7 @@
       </c>
       <c r="J573" s="21"/>
     </row>
-    <row r="574" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A574" s="20">
         <v>32003711</v>
       </c>
@@ -20113,7 +20112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="577" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A577" s="20">
         <v>82000127</v>
       </c>
@@ -20143,7 +20142,7 @@
       </c>
       <c r="J577" s="21"/>
     </row>
-    <row r="578" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A578" s="20">
         <v>82000127</v>
       </c>
@@ -20294,91 +20293,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J582" xr:uid="{80D742BF-D277-4657-84BB-A3DD0282270A}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="12001601"/>
-        <filter val="12002001"/>
-        <filter val="12002401"/>
-        <filter val="12005101"/>
-        <filter val="12007101"/>
-        <filter val="13020301"/>
-        <filter val="13115701"/>
-        <filter val="13116801"/>
-        <filter val="17000101"/>
-        <filter val="22003301"/>
-        <filter val="22003601"/>
-        <filter val="22003701"/>
-        <filter val="22003901"/>
-        <filter val="22010501"/>
-        <filter val="22112501"/>
-        <filter val="22113101"/>
-        <filter val="24000701"/>
-        <filter val="25001201"/>
-        <filter val="25006101"/>
-        <filter val="25017301"/>
-        <filter val="25018501"/>
-        <filter val="25117001"/>
-        <filter val="25117701"/>
-        <filter val="32003201"/>
-        <filter val="33001301"/>
-        <filter val="41007201"/>
-        <filter val="41013901"/>
-        <filter val="41016501"/>
-        <filter val="41017201"/>
-        <filter val="41035201"/>
-        <filter val="41040801"/>
-        <filter val="42006301"/>
-        <filter val="43010901"/>
-        <filter val="43013801"/>
-        <filter val="43127601"/>
-        <filter val="43132201"/>
-        <filter val="51005601"/>
-        <filter val="51005801"/>
-        <filter val="51007201"/>
-        <filter val="51011101"/>
-        <filter val="51011201"/>
-        <filter val="51011301"/>
-        <filter val="51012901"/>
-        <filter val="51034001"/>
-        <filter val="51035401"/>
-        <filter val="51036201"/>
-        <filter val="51036901"/>
-        <filter val="51037201"/>
-        <filter val="51037301"/>
-        <filter val="51039101"/>
-        <filter val="51040001"/>
-        <filter val="51040201"/>
-        <filter val="51041501"/>
-        <filter val="51041801"/>
-        <filter val="51042901"/>
-        <filter val="51043001"/>
-        <filter val="51043201"/>
-        <filter val="51053101"/>
-        <filter val="51054401"/>
-        <filter val="51054601"/>
-        <filter val="51054801"/>
-        <filter val="51054901"/>
-        <filter val="51055001"/>
-        <filter val="51056501"/>
-        <filter val="51058601"/>
-        <filter val="51058901"/>
-        <filter val="52000201"/>
-        <filter val="53016001"/>
-        <filter val="54006001"/>
-        <filter val="54006901"/>
-        <filter val="54007401"/>
-        <filter val="54007801"/>
-        <filter val="54007901"/>
-        <filter val="54008001"/>
-        <filter val="54008101"/>
-        <filter val="81041501"/>
-        <filter val="81042901"/>
-        <filter val="91041501"/>
-        <filter val="91042901"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <conditionalFormatting sqref="F1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Need to Check Dynamic Data
</commit_message>
<xml_diff>
--- a/Input/My Logic Excel.xlsx
+++ b/Input/My Logic Excel.xlsx
@@ -8,28 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\UiPath\SodexoProcess\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5328835-8E30-4960-9268-3F44ED40131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4077CA56-C818-4C67-BC12-DE10EEDB0F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Sheet'!$A$1:$J$582</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="0">'Main Sheet'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="804">
   <si>
     <t>PC Code</t>
   </si>
@@ -2348,13 +2360,106 @@
   </si>
   <si>
     <t xml:space="preserve">RCM ON RENT </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gaurav1</t>
+  </si>
+  <si>
+    <t>Gaurav2</t>
+  </si>
+  <si>
+    <t>Gaurav3</t>
+  </si>
+  <si>
+    <t>Gaurav4</t>
+  </si>
+  <si>
+    <t>Gaurav5</t>
+  </si>
+  <si>
+    <t>Gaurav6</t>
+  </si>
+  <si>
+    <t>Gaurav7</t>
+  </si>
+  <si>
+    <t>Gaurav8</t>
+  </si>
+  <si>
+    <t>Gaurav9</t>
+  </si>
+  <si>
+    <t>Mumbai1</t>
+  </si>
+  <si>
+    <t>Mumbai2</t>
+  </si>
+  <si>
+    <t>Mumbai3</t>
+  </si>
+  <si>
+    <t>Mumbai4</t>
+  </si>
+  <si>
+    <t>Mumbai5</t>
+  </si>
+  <si>
+    <t>Mumbai6</t>
+  </si>
+  <si>
+    <t>Mumbai7</t>
+  </si>
+  <si>
+    <t>Mumbai8</t>
+  </si>
+  <si>
+    <t>Mumbai9</t>
+  </si>
+  <si>
+    <t>Gamail1</t>
+  </si>
+  <si>
+    <t>Gamail2</t>
+  </si>
+  <si>
+    <t>Gamail3</t>
+  </si>
+  <si>
+    <t>Gamail4</t>
+  </si>
+  <si>
+    <t>Gamail5</t>
+  </si>
+  <si>
+    <t>Gamail6</t>
+  </si>
+  <si>
+    <t>Gamail7</t>
+  </si>
+  <si>
+    <t>Gamail8</t>
+  </si>
+  <si>
+    <t>Gamail9</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2380,6 +2485,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2450,7 +2561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2517,6 +2628,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2812,8 +2926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D742BF-D277-4657-84BB-A3DD0282270A}">
   <dimension ref="A1:J582"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20304,4 +20418,231 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F76C4D6-179A-49E7-8FD8-769414F3B5FD}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>775</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>776</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>777</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>786</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>795</v>
+      </c>
+      <c r="D3" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>778</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>787</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>796</v>
+      </c>
+      <c r="D4" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>779</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>788</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>797</v>
+      </c>
+      <c r="D5" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>780</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>789</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>798</v>
+      </c>
+      <c r="D6" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>790</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>799</v>
+      </c>
+      <c r="D7" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>791</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>800</v>
+      </c>
+      <c r="D8" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>792</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>801</v>
+      </c>
+      <c r="D9" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>784</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>793</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="D10" s="23">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A42A5A-DB01-4B4B-B2E7-6C61E93CF680}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>775</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>777</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>786</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>790</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>799</v>
+      </c>
+      <c r="D3" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>792</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>801</v>
+      </c>
+      <c r="D4" s="23">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>